<commit_message>
Finished the second part of the work: added the graph folder and the analysis for the themes. The nextand final step will be works on components analysis and a focus on some test. That could also be interesting to add a point on countries of respondants
</commit_message>
<xml_diff>
--- a/base_finale.xlsx
+++ b/base_finale.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="529">
   <si>
     <t xml:space="preserve">mail</t>
   </si>
@@ -1408,6 +1408,18 @@
   </si>
   <si>
     <t xml:space="preserve">6 7 8 9 11 12 13 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pierreyvon7@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 3 5 10 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anamingcrepin5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 8 12 13 15</t>
   </si>
   <si>
     <t xml:space="preserve">hkboboroto@gmail.com</t>
@@ -15477,9 +15489,7 @@
       <c r="C191" t="s">
         <v>466</v>
       </c>
-      <c r="D191" t="s">
-        <v>467</v>
-      </c>
+      <c r="D191"/>
       <c r="E191" t="s">
         <v>37</v>
       </c>
@@ -15489,21 +15499,23 @@
       <c r="G191" t="s">
         <v>29</v>
       </c>
-      <c r="H191"/>
+      <c r="H191" t="s">
+        <v>340</v>
+      </c>
       <c r="I191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J191" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L191" t="n">
         <v>0</v>
       </c>
       <c r="M191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N191" t="n">
         <v>0</v>
@@ -15518,7 +15530,7 @@
         <v>0</v>
       </c>
       <c r="R191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S191" t="n">
         <v>0</v>
@@ -15530,36 +15542,38 @@
         <v>0</v>
       </c>
       <c r="V191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W191" t="s">
         <v>39</v>
       </c>
       <c r="X191" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
+        <v>467</v>
+      </c>
+      <c r="B192" t="n">
+        <v>0</v>
+      </c>
+      <c r="C192" t="s">
         <v>468</v>
-      </c>
-      <c r="B192" t="n">
-        <v>0</v>
-      </c>
-      <c r="C192" t="s">
-        <v>469</v>
       </c>
       <c r="D192"/>
       <c r="E192" t="s">
-        <v>470</v>
+        <v>37</v>
       </c>
       <c r="F192" t="s">
         <v>46</v>
       </c>
       <c r="G192" t="s">
-        <v>92</v>
-      </c>
-      <c r="H192"/>
+        <v>29</v>
+      </c>
+      <c r="H192" t="s">
+        <v>340</v>
+      </c>
       <c r="I192" t="n">
         <v>0</v>
       </c>
@@ -15570,28 +15584,28 @@
         <v>0</v>
       </c>
       <c r="L192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M192" t="n">
         <v>1</v>
       </c>
       <c r="N192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P192" t="n">
         <v>1</v>
       </c>
       <c r="Q192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R192" t="n">
         <v>0</v>
       </c>
       <c r="S192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T192" t="n">
         <v>1</v>
@@ -15606,24 +15620,24 @@
         <v>39</v>
       </c>
       <c r="X192" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
+        <v>469</v>
+      </c>
+      <c r="B193" t="n">
+        <v>0</v>
+      </c>
+      <c r="C193" t="s">
+        <v>470</v>
+      </c>
+      <c r="D193" t="s">
         <v>471</v>
       </c>
-      <c r="B193" t="n">
-        <v>0</v>
-      </c>
-      <c r="C193" t="s">
-        <v>472</v>
-      </c>
-      <c r="D193" t="s">
-        <v>26</v>
-      </c>
       <c r="E193" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F193" t="s">
         <v>46</v>
@@ -15633,10 +15647,10 @@
       </c>
       <c r="H193"/>
       <c r="I193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K193" t="n">
         <v>0</v>
@@ -15645,19 +15659,19 @@
         <v>0</v>
       </c>
       <c r="M193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N193" t="n">
         <v>0</v>
       </c>
       <c r="O193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P193" t="n">
         <v>0</v>
       </c>
       <c r="Q193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R193" t="n">
         <v>0</v>
@@ -15672,38 +15686,38 @@
         <v>0</v>
       </c>
       <c r="V193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W193" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="X193" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
+        <v>472</v>
+      </c>
+      <c r="B194" t="n">
+        <v>0</v>
+      </c>
+      <c r="C194" t="s">
         <v>473</v>
-      </c>
-      <c r="B194" t="n">
-        <v>0</v>
-      </c>
-      <c r="C194" t="s">
-        <v>474</v>
       </c>
       <c r="D194"/>
       <c r="E194" t="s">
-        <v>42</v>
+        <v>474</v>
       </c>
       <c r="F194" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G194" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="H194"/>
       <c r="I194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J194" t="n">
         <v>0</v>
@@ -15712,13 +15726,13 @@
         <v>0</v>
       </c>
       <c r="L194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M194" t="n">
         <v>1</v>
       </c>
       <c r="N194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O194" t="n">
         <v>1</v>
@@ -15727,28 +15741,28 @@
         <v>1</v>
       </c>
       <c r="Q194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V194" t="n">
         <v>0</v>
       </c>
       <c r="W194" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="X194" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="195">
@@ -15759,17 +15773,19 @@
         <v>0</v>
       </c>
       <c r="C195" t="s">
-        <v>45</v>
-      </c>
-      <c r="D195"/>
+        <v>476</v>
+      </c>
+      <c r="D195" t="s">
+        <v>26</v>
+      </c>
       <c r="E195" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="F195" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G195" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H195"/>
       <c r="I195" t="n">
@@ -15779,7 +15795,7 @@
         <v>0</v>
       </c>
       <c r="K195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L195" t="n">
         <v>0</v>
@@ -15788,16 +15804,16 @@
         <v>1</v>
       </c>
       <c r="N195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P195" t="n">
         <v>0</v>
       </c>
       <c r="Q195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R195" t="n">
         <v>0</v>
@@ -15815,7 +15831,7 @@
         <v>1</v>
       </c>
       <c r="W195" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="X195" t="n">
         <v>5</v>
@@ -15823,21 +15839,27 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B196" t="n">
         <v>0</v>
       </c>
-      <c r="C196"/>
+      <c r="C196" t="s">
+        <v>478</v>
+      </c>
       <c r="D196"/>
-      <c r="E196"/>
-      <c r="F196"/>
+      <c r="E196" t="s">
+        <v>42</v>
+      </c>
+      <c r="F196" t="s">
+        <v>28</v>
+      </c>
       <c r="G196" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="H196"/>
       <c r="I196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J196" t="n">
         <v>0</v>
@@ -15849,22 +15871,22 @@
         <v>0</v>
       </c>
       <c r="M196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N196" t="n">
         <v>0</v>
       </c>
       <c r="O196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q196" t="n">
         <v>0</v>
       </c>
       <c r="R196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S196" t="n">
         <v>0</v>
@@ -15878,61 +15900,63 @@
       <c r="V196" t="n">
         <v>0</v>
       </c>
-      <c r="W196"/>
+      <c r="W196" t="s">
+        <v>43</v>
+      </c>
       <c r="X196" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B197" t="n">
         <v>0</v>
       </c>
       <c r="C197" t="s">
-        <v>478</v>
+        <v>45</v>
       </c>
       <c r="D197"/>
       <c r="E197" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F197" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G197" t="s">
         <v>38</v>
       </c>
       <c r="H197"/>
       <c r="I197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J197" t="n">
         <v>0</v>
       </c>
       <c r="K197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L197" t="n">
         <v>0</v>
       </c>
       <c r="M197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O197" t="n">
         <v>0</v>
       </c>
       <c r="P197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q197" t="n">
         <v>0</v>
       </c>
       <c r="R197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S197" t="n">
         <v>0</v>
@@ -15947,40 +15971,32 @@
         <v>1</v>
       </c>
       <c r="W197" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="X197" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B198" t="n">
         <v>0</v>
       </c>
-      <c r="C198" t="s">
-        <v>480</v>
-      </c>
+      <c r="C198"/>
       <c r="D198"/>
-      <c r="E198" t="s">
-        <v>78</v>
-      </c>
-      <c r="F198" t="s">
-        <v>28</v>
-      </c>
+      <c r="E198"/>
+      <c r="F198"/>
       <c r="G198" t="s">
-        <v>38</v>
-      </c>
-      <c r="H198" t="s">
-        <v>340</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="H198"/>
       <c r="I198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K198" t="n">
         <v>0</v>
@@ -15989,7 +16005,7 @@
         <v>0</v>
       </c>
       <c r="M198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N198" t="n">
         <v>0</v>
@@ -16001,7 +16017,7 @@
         <v>0</v>
       </c>
       <c r="Q198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R198" t="n">
         <v>0</v>
@@ -16010,19 +16026,17 @@
         <v>0</v>
       </c>
       <c r="T198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U198" t="n">
         <v>0</v>
       </c>
       <c r="V198" t="n">
-        <v>1</v>
-      </c>
-      <c r="W198" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W198"/>
       <c r="X198" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -16037,22 +16051,20 @@
       </c>
       <c r="D199"/>
       <c r="E199" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="F199" t="s">
         <v>46</v>
       </c>
       <c r="G199" t="s">
-        <v>92</v>
-      </c>
-      <c r="H199" t="s">
-        <v>340</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H199"/>
       <c r="I199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K199" t="n">
         <v>0</v>
@@ -16061,22 +16073,22 @@
         <v>0</v>
       </c>
       <c r="M199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O199" t="n">
         <v>0</v>
       </c>
       <c r="P199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S199" t="n">
         <v>0</v>
@@ -16088,13 +16100,13 @@
         <v>0</v>
       </c>
       <c r="V199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W199" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="X199" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200">
@@ -16107,24 +16119,24 @@
       <c r="C200" t="s">
         <v>484</v>
       </c>
-      <c r="D200" t="s">
-        <v>485</v>
-      </c>
+      <c r="D200"/>
       <c r="E200" t="s">
-        <v>486</v>
+        <v>78</v>
       </c>
       <c r="F200" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G200" t="s">
-        <v>29</v>
-      </c>
-      <c r="H200"/>
+        <v>38</v>
+      </c>
+      <c r="H200" t="s">
+        <v>340</v>
+      </c>
       <c r="I200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K200" t="n">
         <v>0</v>
@@ -16142,7 +16154,7 @@
         <v>0</v>
       </c>
       <c r="P200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q200" t="n">
         <v>1</v>
@@ -16154,7 +16166,7 @@
         <v>0</v>
       </c>
       <c r="T200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U200" t="n">
         <v>0</v>
@@ -16163,55 +16175,55 @@
         <v>1</v>
       </c>
       <c r="W200" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="X200" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B201" t="n">
         <v>0</v>
       </c>
       <c r="C201" t="s">
-        <v>488</v>
-      </c>
-      <c r="D201" t="s">
-        <v>489</v>
-      </c>
+        <v>486</v>
+      </c>
+      <c r="D201"/>
       <c r="E201" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="F201" t="s">
         <v>46</v>
       </c>
       <c r="G201" t="s">
-        <v>29</v>
-      </c>
-      <c r="H201"/>
+        <v>92</v>
+      </c>
+      <c r="H201" t="s">
+        <v>340</v>
+      </c>
       <c r="I201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K201" t="n">
         <v>0</v>
       </c>
       <c r="L201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P201" t="n">
         <v>0</v>
@@ -16220,13 +16232,13 @@
         <v>1</v>
       </c>
       <c r="R201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S201" t="n">
         <v>0</v>
       </c>
       <c r="T201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U201" t="n">
         <v>0</v>
@@ -16235,7 +16247,7 @@
         <v>0</v>
       </c>
       <c r="W201" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="X201" t="n">
         <v>5</v>
@@ -16243,25 +16255,25 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
+        <v>487</v>
+      </c>
+      <c r="B202" t="n">
+        <v>0</v>
+      </c>
+      <c r="C202" t="s">
+        <v>488</v>
+      </c>
+      <c r="D202" t="s">
+        <v>489</v>
+      </c>
+      <c r="E202" t="s">
         <v>490</v>
       </c>
-      <c r="B202" t="n">
-        <v>0</v>
-      </c>
-      <c r="C202" t="s">
-        <v>491</v>
-      </c>
-      <c r="D202" t="s">
-        <v>26</v>
-      </c>
-      <c r="E202" t="s">
-        <v>492</v>
-      </c>
       <c r="F202" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G202" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H202"/>
       <c r="I202" t="n">
@@ -16274,22 +16286,22 @@
         <v>0</v>
       </c>
       <c r="L202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M202" t="n">
         <v>1</v>
       </c>
       <c r="N202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R202" t="n">
         <v>0</v>
@@ -16304,10 +16316,10 @@
         <v>0</v>
       </c>
       <c r="V202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W202" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="X202" t="n">
         <v>4</v>
@@ -16315,38 +16327,38 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
+        <v>491</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0</v>
+      </c>
+      <c r="C203" t="s">
+        <v>492</v>
+      </c>
+      <c r="D203" t="s">
         <v>493</v>
       </c>
-      <c r="B203" t="n">
-        <v>0</v>
-      </c>
-      <c r="C203" t="s">
-        <v>494</v>
-      </c>
-      <c r="D203" t="s">
-        <v>495</v>
-      </c>
       <c r="E203" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F203" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G203" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H203"/>
       <c r="I203" t="n">
         <v>0</v>
       </c>
       <c r="J203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M203" t="n">
         <v>0</v>
@@ -16355,7 +16367,7 @@
         <v>0</v>
       </c>
       <c r="O203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P203" t="n">
         <v>0</v>
@@ -16364,7 +16376,7 @@
         <v>1</v>
       </c>
       <c r="R203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S203" t="n">
         <v>0</v>
@@ -16379,35 +16391,37 @@
         <v>0</v>
       </c>
       <c r="W203" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="X203" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
+        <v>494</v>
+      </c>
+      <c r="B204" t="n">
+        <v>0</v>
+      </c>
+      <c r="C204" t="s">
+        <v>495</v>
+      </c>
+      <c r="D204" t="s">
+        <v>26</v>
+      </c>
+      <c r="E204" t="s">
         <v>496</v>
       </c>
-      <c r="B204" t="n">
-        <v>0</v>
-      </c>
-      <c r="C204" t="s">
-        <v>497</v>
-      </c>
-      <c r="D204"/>
-      <c r="E204" t="s">
-        <v>56</v>
-      </c>
       <c r="F204" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G204" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="H204"/>
       <c r="I204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J204" t="n">
         <v>0</v>
@@ -16416,10 +16430,10 @@
         <v>0</v>
       </c>
       <c r="L204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N204" t="n">
         <v>1</v>
@@ -16434,13 +16448,13 @@
         <v>0</v>
       </c>
       <c r="R204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S204" t="n">
         <v>0</v>
       </c>
       <c r="T204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U204" t="n">
         <v>0</v>
@@ -16449,9 +16463,151 @@
         <v>0</v>
       </c>
       <c r="W204" t="s">
+        <v>50</v>
+      </c>
+      <c r="X204" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>497</v>
+      </c>
+      <c r="B205" t="n">
+        <v>0</v>
+      </c>
+      <c r="C205" t="s">
+        <v>498</v>
+      </c>
+      <c r="D205" t="s">
+        <v>499</v>
+      </c>
+      <c r="E205" t="s">
+        <v>37</v>
+      </c>
+      <c r="F205" t="s">
+        <v>28</v>
+      </c>
+      <c r="G205" t="s">
+        <v>38</v>
+      </c>
+      <c r="H205"/>
+      <c r="I205" t="n">
+        <v>0</v>
+      </c>
+      <c r="J205" t="n">
+        <v>1</v>
+      </c>
+      <c r="K205" t="n">
+        <v>1</v>
+      </c>
+      <c r="L205" t="n">
+        <v>0</v>
+      </c>
+      <c r="M205" t="n">
+        <v>0</v>
+      </c>
+      <c r="N205" t="n">
+        <v>0</v>
+      </c>
+      <c r="O205" t="n">
+        <v>0</v>
+      </c>
+      <c r="P205" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q205" t="n">
+        <v>1</v>
+      </c>
+      <c r="R205" t="n">
+        <v>0</v>
+      </c>
+      <c r="S205" t="n">
+        <v>0</v>
+      </c>
+      <c r="T205" t="n">
+        <v>1</v>
+      </c>
+      <c r="U205" t="n">
+        <v>0</v>
+      </c>
+      <c r="V205" t="n">
+        <v>0</v>
+      </c>
+      <c r="W205" t="s">
+        <v>39</v>
+      </c>
+      <c r="X205" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>500</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0</v>
+      </c>
+      <c r="C206" t="s">
+        <v>501</v>
+      </c>
+      <c r="D206"/>
+      <c r="E206" t="s">
+        <v>56</v>
+      </c>
+      <c r="F206" t="s">
+        <v>46</v>
+      </c>
+      <c r="G206" t="s">
+        <v>92</v>
+      </c>
+      <c r="H206"/>
+      <c r="I206" t="n">
+        <v>1</v>
+      </c>
+      <c r="J206" t="n">
+        <v>0</v>
+      </c>
+      <c r="K206" t="n">
+        <v>0</v>
+      </c>
+      <c r="L206" t="n">
+        <v>0</v>
+      </c>
+      <c r="M206" t="n">
+        <v>0</v>
+      </c>
+      <c r="N206" t="n">
+        <v>1</v>
+      </c>
+      <c r="O206" t="n">
+        <v>1</v>
+      </c>
+      <c r="P206" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q206" t="n">
+        <v>0</v>
+      </c>
+      <c r="R206" t="n">
+        <v>1</v>
+      </c>
+      <c r="S206" t="n">
+        <v>0</v>
+      </c>
+      <c r="T206" t="n">
+        <v>1</v>
+      </c>
+      <c r="U206" t="n">
+        <v>0</v>
+      </c>
+      <c r="V206" t="n">
+        <v>0</v>
+      </c>
+      <c r="W206" t="s">
         <v>57</v>
       </c>
-      <c r="X204" t="n">
+      <c r="X206" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16471,15 +16627,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B3" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4">
@@ -16487,7 +16643,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
     <row r="5">
@@ -16495,7 +16651,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6">
@@ -16503,7 +16659,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7">
@@ -16511,7 +16667,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="8">
@@ -16519,7 +16675,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9">
@@ -16527,7 +16683,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="10">
@@ -16535,7 +16691,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
     </row>
     <row r="11">
@@ -16543,7 +16699,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="12">
@@ -16551,7 +16707,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="13">
@@ -16559,7 +16715,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
     </row>
     <row r="14">
@@ -16567,7 +16723,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="15">
@@ -16575,7 +16731,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
     </row>
     <row r="16">
@@ -16583,7 +16739,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17">
@@ -16591,7 +16747,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18">
@@ -16599,7 +16755,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
     </row>
     <row r="19">
@@ -16607,7 +16763,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
     <row r="20">
@@ -16615,7 +16771,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="21">
@@ -16623,7 +16779,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
     </row>
     <row r="22">
@@ -16631,7 +16787,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="23">
@@ -16639,7 +16795,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
     </row>
     <row r="24">
@@ -16647,7 +16803,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="25">
@@ -16655,7 +16811,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
     </row>
     <row r="26">
@@ -16663,7 +16819,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="27">
@@ -16671,7 +16827,7 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final part of the analysis, I think the work is over and I will not add something new.
</commit_message>
<xml_diff>
--- a/base_finale.xlsx
+++ b/base_finale.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="539">
   <si>
     <t xml:space="preserve">mail</t>
   </si>
@@ -1422,6 +1422,36 @@
     <t xml:space="preserve">5 8 12 13 15</t>
   </si>
   <si>
+    <t xml:space="preserve">atchocharlotte@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 5 6 7 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les communications telephoniques sont securisees a combien de pourcentage ? que ce soit appels normaux ou sur les reseaux sociaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julestnk41@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 8 11 13 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la conception de logiciels et de materiel informatique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assiba@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marketing digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hadefoulou@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 4 8 13 14 15</t>
+  </si>
+  <si>
     <t xml:space="preserve">hkboboroto@gmail.com</t>
   </si>
   <si>
@@ -1530,7 +1560,7 @@
     <t xml:space="preserve">labels</t>
   </si>
   <si>
-    <t xml:space="preserve">mails des repondants</t>
+    <t xml:space="preserve">mails des répondants</t>
   </si>
   <si>
     <t xml:space="preserve">score</t>
@@ -15637,20 +15667,22 @@
         <v>471</v>
       </c>
       <c r="E193" t="s">
-        <v>37</v>
+        <v>365</v>
       </c>
       <c r="F193" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G193" t="s">
-        <v>29</v>
-      </c>
-      <c r="H193"/>
+        <v>38</v>
+      </c>
+      <c r="H193" t="s">
+        <v>449</v>
+      </c>
       <c r="I193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K193" t="n">
         <v>0</v>
@@ -15659,19 +15691,19 @@
         <v>0</v>
       </c>
       <c r="M193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P193" t="n">
         <v>0</v>
       </c>
       <c r="Q193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R193" t="n">
         <v>0</v>
@@ -15689,10 +15721,10 @@
         <v>0</v>
       </c>
       <c r="W193" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="X193" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194">
@@ -15705,17 +15737,21 @@
       <c r="C194" t="s">
         <v>473</v>
       </c>
-      <c r="D194"/>
+      <c r="D194" t="s">
+        <v>474</v>
+      </c>
       <c r="E194" t="s">
-        <v>474</v>
+        <v>42</v>
       </c>
       <c r="F194" t="s">
         <v>46</v>
       </c>
       <c r="G194" t="s">
-        <v>92</v>
-      </c>
-      <c r="H194"/>
+        <v>38</v>
+      </c>
+      <c r="H194" t="s">
+        <v>449</v>
+      </c>
       <c r="I194" t="n">
         <v>0</v>
       </c>
@@ -15726,13 +15762,13 @@
         <v>0</v>
       </c>
       <c r="L194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O194" t="n">
         <v>1</v>
@@ -15741,7 +15777,7 @@
         <v>1</v>
       </c>
       <c r="Q194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R194" t="n">
         <v>0</v>
@@ -15750,19 +15786,19 @@
         <v>1</v>
       </c>
       <c r="T194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U194" t="n">
         <v>1</v>
       </c>
       <c r="V194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W194" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="X194" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195">
@@ -15773,32 +15809,34 @@
         <v>0</v>
       </c>
       <c r="C195" t="s">
+        <v>70</v>
+      </c>
+      <c r="D195" t="s">
         <v>476</v>
       </c>
-      <c r="D195" t="s">
-        <v>26</v>
-      </c>
       <c r="E195" t="s">
-        <v>56</v>
+        <v>365</v>
       </c>
       <c r="F195" t="s">
         <v>46</v>
       </c>
       <c r="G195" t="s">
-        <v>29</v>
-      </c>
-      <c r="H195"/>
+        <v>92</v>
+      </c>
+      <c r="H195" t="s">
+        <v>340</v>
+      </c>
       <c r="I195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J195" t="n">
         <v>0</v>
       </c>
       <c r="K195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M195" t="n">
         <v>1</v>
@@ -15807,13 +15845,13 @@
         <v>0</v>
       </c>
       <c r="O195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P195" t="n">
         <v>0</v>
       </c>
       <c r="Q195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R195" t="n">
         <v>0</v>
@@ -15822,7 +15860,7 @@
         <v>0</v>
       </c>
       <c r="T195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U195" t="n">
         <v>0</v>
@@ -15852,32 +15890,34 @@
         <v>42</v>
       </c>
       <c r="F196" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G196" t="s">
         <v>38</v>
       </c>
-      <c r="H196"/>
+      <c r="H196" t="s">
+        <v>340</v>
+      </c>
       <c r="I196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J196" t="n">
         <v>0</v>
       </c>
       <c r="K196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N196" t="n">
         <v>0</v>
       </c>
       <c r="O196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P196" t="n">
         <v>1</v>
@@ -15886,7 +15926,7 @@
         <v>0</v>
       </c>
       <c r="R196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S196" t="n">
         <v>0</v>
@@ -15895,10 +15935,10 @@
         <v>0</v>
       </c>
       <c r="U196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W196" t="s">
         <v>43</v>
@@ -15915,36 +15955,38 @@
         <v>0</v>
       </c>
       <c r="C197" t="s">
-        <v>45</v>
-      </c>
-      <c r="D197"/>
+        <v>480</v>
+      </c>
+      <c r="D197" t="s">
+        <v>481</v>
+      </c>
       <c r="E197" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F197" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G197" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H197"/>
       <c r="I197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L197" t="n">
         <v>0</v>
       </c>
       <c r="M197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O197" t="n">
         <v>0</v>
@@ -15968,26 +16010,32 @@
         <v>0</v>
       </c>
       <c r="V197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W197" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="X197" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B198" t="n">
         <v>0</v>
       </c>
-      <c r="C198"/>
+      <c r="C198" t="s">
+        <v>483</v>
+      </c>
       <c r="D198"/>
-      <c r="E198"/>
-      <c r="F198"/>
+      <c r="E198" t="s">
+        <v>484</v>
+      </c>
+      <c r="F198" t="s">
+        <v>46</v>
+      </c>
       <c r="G198" t="s">
         <v>92</v>
       </c>
@@ -16002,66 +16050,70 @@
         <v>0</v>
       </c>
       <c r="L198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R198" t="n">
         <v>0</v>
       </c>
       <c r="S198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V198" t="n">
         <v>0</v>
       </c>
-      <c r="W198"/>
+      <c r="W198" t="s">
+        <v>39</v>
+      </c>
       <c r="X198" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B199" t="n">
         <v>0</v>
       </c>
       <c r="C199" t="s">
-        <v>482</v>
-      </c>
-      <c r="D199"/>
+        <v>486</v>
+      </c>
+      <c r="D199" t="s">
+        <v>26</v>
+      </c>
       <c r="E199" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F199" t="s">
         <v>46</v>
       </c>
       <c r="G199" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H199"/>
       <c r="I199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J199" t="n">
         <v>0</v>
@@ -16073,22 +16125,22 @@
         <v>0</v>
       </c>
       <c r="M199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N199" t="n">
         <v>0</v>
       </c>
       <c r="O199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S199" t="n">
         <v>0</v>
@@ -16103,25 +16155,25 @@
         <v>1</v>
       </c>
       <c r="W199" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="X199" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="B200" t="n">
         <v>0</v>
       </c>
       <c r="C200" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="D200"/>
       <c r="E200" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="F200" t="s">
         <v>28</v>
@@ -16129,14 +16181,12 @@
       <c r="G200" t="s">
         <v>38</v>
       </c>
-      <c r="H200" t="s">
-        <v>340</v>
-      </c>
+      <c r="H200"/>
       <c r="I200" t="n">
         <v>1</v>
       </c>
       <c r="J200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K200" t="n">
         <v>0</v>
@@ -16151,67 +16201,65 @@
         <v>0</v>
       </c>
       <c r="O200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S200" t="n">
         <v>0</v>
       </c>
       <c r="T200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U200" t="n">
         <v>0</v>
       </c>
       <c r="V200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W200" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="X200" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B201" t="n">
         <v>0</v>
       </c>
       <c r="C201" t="s">
-        <v>486</v>
+        <v>45</v>
       </c>
       <c r="D201"/>
       <c r="E201" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="F201" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G201" t="s">
-        <v>92</v>
-      </c>
-      <c r="H201" t="s">
-        <v>340</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H201"/>
       <c r="I201" t="n">
         <v>1</v>
       </c>
       <c r="J201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L201" t="n">
         <v>0</v>
@@ -16229,7 +16277,7 @@
         <v>0</v>
       </c>
       <c r="Q201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R201" t="n">
         <v>0</v>
@@ -16244,10 +16292,10 @@
         <v>0</v>
       </c>
       <c r="V201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W201" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="X201" t="n">
         <v>5</v>
@@ -16255,25 +16303,17 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B202" t="n">
         <v>0</v>
       </c>
-      <c r="C202" t="s">
-        <v>488</v>
-      </c>
-      <c r="D202" t="s">
-        <v>489</v>
-      </c>
-      <c r="E202" t="s">
-        <v>490</v>
-      </c>
-      <c r="F202" t="s">
-        <v>46</v>
-      </c>
+      <c r="C202"/>
+      <c r="D202"/>
+      <c r="E202"/>
+      <c r="F202"/>
       <c r="G202" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="H202"/>
       <c r="I202" t="n">
@@ -16289,7 +16329,7 @@
         <v>0</v>
       </c>
       <c r="M202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N202" t="n">
         <v>0</v>
@@ -16298,10 +16338,10 @@
         <v>0</v>
       </c>
       <c r="P202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R202" t="n">
         <v>0</v>
@@ -16316,13 +16356,11 @@
         <v>0</v>
       </c>
       <c r="V202" t="n">
-        <v>1</v>
-      </c>
-      <c r="W202" t="s">
-        <v>27</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W202"/>
       <c r="X202" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -16335,9 +16373,7 @@
       <c r="C203" t="s">
         <v>492</v>
       </c>
-      <c r="D203" t="s">
-        <v>493</v>
-      </c>
+      <c r="D203"/>
       <c r="E203" t="s">
         <v>42</v>
       </c>
@@ -16345,7 +16381,7 @@
         <v>46</v>
       </c>
       <c r="G203" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H203"/>
       <c r="I203" t="n">
@@ -16358,7 +16394,7 @@
         <v>0</v>
       </c>
       <c r="L203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M203" t="n">
         <v>0</v>
@@ -16367,13 +16403,13 @@
         <v>0</v>
       </c>
       <c r="O203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R203" t="n">
         <v>1</v>
@@ -16382,36 +16418,34 @@
         <v>0</v>
       </c>
       <c r="T203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U203" t="n">
         <v>0</v>
       </c>
       <c r="V203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W203" t="s">
         <v>43</v>
       </c>
       <c r="X203" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
+        <v>493</v>
+      </c>
+      <c r="B204" t="n">
+        <v>0</v>
+      </c>
+      <c r="C204" t="s">
         <v>494</v>
       </c>
-      <c r="B204" t="n">
-        <v>0</v>
-      </c>
-      <c r="C204" t="s">
-        <v>495</v>
-      </c>
-      <c r="D204" t="s">
-        <v>26</v>
-      </c>
+      <c r="D204"/>
       <c r="E204" t="s">
-        <v>496</v>
+        <v>78</v>
       </c>
       <c r="F204" t="s">
         <v>28</v>
@@ -16419,33 +16453,35 @@
       <c r="G204" t="s">
         <v>38</v>
       </c>
-      <c r="H204"/>
+      <c r="H204" t="s">
+        <v>340</v>
+      </c>
       <c r="I204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K204" t="n">
         <v>0</v>
       </c>
       <c r="L204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M204" t="n">
         <v>1</v>
       </c>
       <c r="N204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P204" t="n">
         <v>0</v>
       </c>
       <c r="Q204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R204" t="n">
         <v>0</v>
@@ -16454,61 +16490,61 @@
         <v>0</v>
       </c>
       <c r="T204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U204" t="n">
         <v>0</v>
       </c>
       <c r="V204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W204" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="X204" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B205" t="n">
         <v>0</v>
       </c>
       <c r="C205" t="s">
-        <v>498</v>
-      </c>
-      <c r="D205" t="s">
-        <v>499</v>
-      </c>
+        <v>496</v>
+      </c>
+      <c r="D205"/>
       <c r="E205" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="F205" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G205" t="s">
-        <v>38</v>
-      </c>
-      <c r="H205"/>
+        <v>92</v>
+      </c>
+      <c r="H205" t="s">
+        <v>340</v>
+      </c>
       <c r="I205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J205" t="n">
         <v>1</v>
       </c>
       <c r="K205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L205" t="n">
         <v>0</v>
       </c>
       <c r="M205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O205" t="n">
         <v>0</v>
@@ -16526,7 +16562,7 @@
         <v>0</v>
       </c>
       <c r="T205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U205" t="n">
         <v>0</v>
@@ -16535,35 +16571,37 @@
         <v>0</v>
       </c>
       <c r="W205" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="X205" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
+        <v>497</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0</v>
+      </c>
+      <c r="C206" t="s">
+        <v>498</v>
+      </c>
+      <c r="D206" t="s">
+        <v>499</v>
+      </c>
+      <c r="E206" t="s">
         <v>500</v>
-      </c>
-      <c r="B206" t="n">
-        <v>0</v>
-      </c>
-      <c r="C206" t="s">
-        <v>501</v>
-      </c>
-      <c r="D206"/>
-      <c r="E206" t="s">
-        <v>56</v>
       </c>
       <c r="F206" t="s">
         <v>46</v>
       </c>
       <c r="G206" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="H206"/>
       <c r="I206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J206" t="n">
         <v>0</v>
@@ -16575,39 +16613,325 @@
         <v>0</v>
       </c>
       <c r="M206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S206" t="n">
         <v>0</v>
       </c>
       <c r="T206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U206" t="n">
         <v>0</v>
       </c>
       <c r="V206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W206" t="s">
+        <v>27</v>
+      </c>
+      <c r="X206" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>501</v>
+      </c>
+      <c r="B207" t="n">
+        <v>0</v>
+      </c>
+      <c r="C207" t="s">
+        <v>502</v>
+      </c>
+      <c r="D207" t="s">
+        <v>503</v>
+      </c>
+      <c r="E207" t="s">
+        <v>42</v>
+      </c>
+      <c r="F207" t="s">
+        <v>46</v>
+      </c>
+      <c r="G207" t="s">
+        <v>29</v>
+      </c>
+      <c r="H207"/>
+      <c r="I207" t="n">
+        <v>0</v>
+      </c>
+      <c r="J207" t="n">
+        <v>0</v>
+      </c>
+      <c r="K207" t="n">
+        <v>0</v>
+      </c>
+      <c r="L207" t="n">
+        <v>1</v>
+      </c>
+      <c r="M207" t="n">
+        <v>0</v>
+      </c>
+      <c r="N207" t="n">
+        <v>0</v>
+      </c>
+      <c r="O207" t="n">
+        <v>1</v>
+      </c>
+      <c r="P207" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q207" t="n">
+        <v>1</v>
+      </c>
+      <c r="R207" t="n">
+        <v>1</v>
+      </c>
+      <c r="S207" t="n">
+        <v>0</v>
+      </c>
+      <c r="T207" t="n">
+        <v>1</v>
+      </c>
+      <c r="U207" t="n">
+        <v>0</v>
+      </c>
+      <c r="V207" t="n">
+        <v>0</v>
+      </c>
+      <c r="W207" t="s">
+        <v>43</v>
+      </c>
+      <c r="X207" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>504</v>
+      </c>
+      <c r="B208" t="n">
+        <v>0</v>
+      </c>
+      <c r="C208" t="s">
+        <v>505</v>
+      </c>
+      <c r="D208" t="s">
+        <v>26</v>
+      </c>
+      <c r="E208" t="s">
+        <v>506</v>
+      </c>
+      <c r="F208" t="s">
+        <v>28</v>
+      </c>
+      <c r="G208" t="s">
+        <v>38</v>
+      </c>
+      <c r="H208"/>
+      <c r="I208" t="n">
+        <v>0</v>
+      </c>
+      <c r="J208" t="n">
+        <v>0</v>
+      </c>
+      <c r="K208" t="n">
+        <v>0</v>
+      </c>
+      <c r="L208" t="n">
+        <v>1</v>
+      </c>
+      <c r="M208" t="n">
+        <v>1</v>
+      </c>
+      <c r="N208" t="n">
+        <v>1</v>
+      </c>
+      <c r="O208" t="n">
+        <v>1</v>
+      </c>
+      <c r="P208" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q208" t="n">
+        <v>0</v>
+      </c>
+      <c r="R208" t="n">
+        <v>0</v>
+      </c>
+      <c r="S208" t="n">
+        <v>0</v>
+      </c>
+      <c r="T208" t="n">
+        <v>0</v>
+      </c>
+      <c r="U208" t="n">
+        <v>0</v>
+      </c>
+      <c r="V208" t="n">
+        <v>0</v>
+      </c>
+      <c r="W208" t="s">
+        <v>50</v>
+      </c>
+      <c r="X208" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>507</v>
+      </c>
+      <c r="B209" t="n">
+        <v>0</v>
+      </c>
+      <c r="C209" t="s">
+        <v>508</v>
+      </c>
+      <c r="D209" t="s">
+        <v>509</v>
+      </c>
+      <c r="E209" t="s">
+        <v>37</v>
+      </c>
+      <c r="F209" t="s">
+        <v>28</v>
+      </c>
+      <c r="G209" t="s">
+        <v>38</v>
+      </c>
+      <c r="H209"/>
+      <c r="I209" t="n">
+        <v>0</v>
+      </c>
+      <c r="J209" t="n">
+        <v>1</v>
+      </c>
+      <c r="K209" t="n">
+        <v>1</v>
+      </c>
+      <c r="L209" t="n">
+        <v>0</v>
+      </c>
+      <c r="M209" t="n">
+        <v>0</v>
+      </c>
+      <c r="N209" t="n">
+        <v>0</v>
+      </c>
+      <c r="O209" t="n">
+        <v>0</v>
+      </c>
+      <c r="P209" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q209" t="n">
+        <v>1</v>
+      </c>
+      <c r="R209" t="n">
+        <v>0</v>
+      </c>
+      <c r="S209" t="n">
+        <v>0</v>
+      </c>
+      <c r="T209" t="n">
+        <v>1</v>
+      </c>
+      <c r="U209" t="n">
+        <v>0</v>
+      </c>
+      <c r="V209" t="n">
+        <v>0</v>
+      </c>
+      <c r="W209" t="s">
+        <v>39</v>
+      </c>
+      <c r="X209" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>510</v>
+      </c>
+      <c r="B210" t="n">
+        <v>0</v>
+      </c>
+      <c r="C210" t="s">
+        <v>511</v>
+      </c>
+      <c r="D210"/>
+      <c r="E210" t="s">
+        <v>56</v>
+      </c>
+      <c r="F210" t="s">
+        <v>46</v>
+      </c>
+      <c r="G210" t="s">
+        <v>92</v>
+      </c>
+      <c r="H210"/>
+      <c r="I210" t="n">
+        <v>1</v>
+      </c>
+      <c r="J210" t="n">
+        <v>0</v>
+      </c>
+      <c r="K210" t="n">
+        <v>0</v>
+      </c>
+      <c r="L210" t="n">
+        <v>0</v>
+      </c>
+      <c r="M210" t="n">
+        <v>0</v>
+      </c>
+      <c r="N210" t="n">
+        <v>1</v>
+      </c>
+      <c r="O210" t="n">
+        <v>1</v>
+      </c>
+      <c r="P210" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q210" t="n">
+        <v>0</v>
+      </c>
+      <c r="R210" t="n">
+        <v>1</v>
+      </c>
+      <c r="S210" t="n">
+        <v>0</v>
+      </c>
+      <c r="T210" t="n">
+        <v>1</v>
+      </c>
+      <c r="U210" t="n">
+        <v>0</v>
+      </c>
+      <c r="V210" t="n">
+        <v>0</v>
+      </c>
+      <c r="W210" t="s">
         <v>57</v>
       </c>
-      <c r="X206" t="n">
+      <c r="X210" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16627,15 +16951,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>502</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="B3" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4">
@@ -16643,7 +16967,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>505</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5">
@@ -16651,7 +16975,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
     </row>
     <row r="6">
@@ -16659,7 +16983,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>507</v>
+        <v>517</v>
       </c>
     </row>
     <row r="7">
@@ -16667,7 +16991,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>508</v>
+        <v>518</v>
       </c>
     </row>
     <row r="8">
@@ -16675,7 +16999,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>509</v>
+        <v>519</v>
       </c>
     </row>
     <row r="9">
@@ -16683,7 +17007,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
     </row>
     <row r="10">
@@ -16691,7 +17015,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
     </row>
     <row r="11">
@@ -16699,7 +17023,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>512</v>
+        <v>522</v>
       </c>
     </row>
     <row r="12">
@@ -16707,7 +17031,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>513</v>
+        <v>523</v>
       </c>
     </row>
     <row r="13">
@@ -16715,7 +17039,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>514</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14">
@@ -16723,7 +17047,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>515</v>
+        <v>525</v>
       </c>
     </row>
     <row r="15">
@@ -16731,7 +17055,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>516</v>
+        <v>526</v>
       </c>
     </row>
     <row r="16">
@@ -16739,7 +17063,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>517</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17">
@@ -16747,7 +17071,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
     </row>
     <row r="18">
@@ -16755,7 +17079,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
     </row>
     <row r="19">
@@ -16763,7 +17087,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
     </row>
     <row r="20">
@@ -16771,7 +17095,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
     </row>
     <row r="21">
@@ -16779,7 +17103,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>522</v>
+        <v>532</v>
       </c>
     </row>
     <row r="22">
@@ -16787,7 +17111,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>523</v>
+        <v>533</v>
       </c>
     </row>
     <row r="23">
@@ -16795,7 +17119,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>524</v>
+        <v>534</v>
       </c>
     </row>
     <row r="24">
@@ -16803,7 +17127,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>525</v>
+        <v>535</v>
       </c>
     </row>
     <row r="25">
@@ -16811,7 +17135,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>526</v>
+        <v>536</v>
       </c>
     </row>
     <row r="26">
@@ -16819,7 +17143,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>527</v>
+        <v>537</v>
       </c>
     </row>
     <row r="27">
@@ -16827,7 +17151,7 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>